<commit_message>
Atualização dos gráficos Burndown
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos Burndown/8ª Sprint/Gráfico Burndown 8.xlsx
+++ b/Documentação/Gráficos Burndown/8ª Sprint/Gráfico Burndown 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cerberus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADAC3B1A-9564-4D0E-98B4-693C37158D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E50A36A5-5EF2-4E3C-9ED3-EF1D98EB1D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
   </bookViews>
@@ -570,9 +570,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,35 +615,38 @@
     <xf numFmtId="1" fontId="4" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,28 +804,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,29 +918,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>31</c:v>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.45</c:v>
+                  <c:v>25.714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.9</c:v>
+                  <c:v>21.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.349999999999998</c:v>
+                  <c:v>17.142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.799999999999997</c:v>
+                  <c:v>12.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.249999999999996</c:v>
+                  <c:v>8.5714285714285765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.699999999999996</c:v>
+                  <c:v>4.2857142857142909</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.149999999999995</c:v>
+                  <c:v>5.3290705182007514E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,28 +1378,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,29 +1541,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>31</c:v>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.45</c:v>
+                  <c:v>25.714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.9</c:v>
+                  <c:v>21.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.349999999999998</c:v>
+                  <c:v>17.142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.799999999999997</c:v>
+                  <c:v>12.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.249999999999996</c:v>
+                  <c:v>8.5714285714285765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.699999999999996</c:v>
+                  <c:v>4.2857142857142909</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.149999999999995</c:v>
+                  <c:v>5.3290705182007514E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3376,7 +3376,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -3390,90 +3390,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:11" ht="97.5" customHeight="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="45.75" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -3503,7 +3503,7 @@
       <c r="I7" s="1">
         <v>7</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -3514,33 +3514,33 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>7</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>2</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>1</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>2</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>1</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16">
+      <c r="G8" s="14"/>
+      <c r="H8" s="15">
         <v>1</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <v>1</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <f>B8-SUM(C8:I8)</f>
         <v>-1</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <f>IFERROR(1-(J8/B8),"")</f>
         <v>1.1428571428571428</v>
       </c>
@@ -3549,25 +3549,25 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>4</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="17">
         <v>2</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>2</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="21">
+      <c r="I9" s="17"/>
+      <c r="J9" s="20">
         <f>B9-SUM(C9:I9)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <f>IFERROR(1-(J9/B9),"")</f>
         <v>1</v>
       </c>
@@ -3576,29 +3576,29 @@
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>4</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>1</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>1</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19">
+      <c r="E10" s="17"/>
+      <c r="F10" s="18">
         <v>1</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19">
+      <c r="G10" s="17"/>
+      <c r="H10" s="18">
         <v>1</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="21">
+      <c r="I10" s="17"/>
+      <c r="J10" s="20">
         <f>B10-SUM(C10:I10)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="12">
         <f>IFERROR(1-(J10/B10),"")</f>
         <v>1</v>
       </c>
@@ -3607,29 +3607,29 @@
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>4</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>1</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>1</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19">
+      <c r="E11" s="17"/>
+      <c r="F11" s="18">
         <v>1</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>2</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="21">
+      <c r="H11" s="18"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="20">
         <f>B11-SUM(C11:I11)</f>
         <v>-1</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="12">
         <f>IFERROR(1-(J11/B11),"")</f>
         <v>1.25</v>
       </c>
@@ -3638,25 +3638,25 @@
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>3</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>1</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="21">
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="20">
         <f>B12-SUM(C12:I12)</f>
         <v>1</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="12">
         <f>IFERROR(1-(J12/B12),"")</f>
         <v>0.66666666666666674</v>
       </c>
@@ -3665,27 +3665,27 @@
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>4</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17"/>
+      <c r="D13" s="18">
         <v>1</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18">
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="17">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="H13" s="18">
         <v>1</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="21">
+      <c r="I13" s="17"/>
+      <c r="J13" s="20">
         <f>B13-SUM(C13:I13)</f>
         <v>1</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="12">
         <f>IFERROR(1-(J13/B13),"")</f>
         <v>0.75</v>
       </c>
@@ -3694,25 +3694,25 @@
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>2</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>1</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="21">
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="20">
         <f>B14-SUM(C14:I14)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="12">
         <f>IFERROR(1-(J14/B14),"")</f>
         <v>1</v>
       </c>
@@ -3721,29 +3721,29 @@
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="17">
-        <v>3</v>
-      </c>
-      <c r="C15" s="18">
+      <c r="B15" s="16">
+        <v>2</v>
+      </c>
+      <c r="C15" s="17">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>1</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>1</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="21">
+      <c r="F15" s="18"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="20">
         <f>B15-SUM(C15:I15)</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K15" s="12">
         <f>IFERROR(1-(J15/B15),"")</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="B16" s="8">
         <f>SUM(B8:B15)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="9">
         <f>IFERROR(IF(B16-SUM(C8:C15)=B16,NA(),B16-SUM(C8:C15)),NA())</f>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="D16" s="9">
         <f>IFERROR(IF(C16-SUM(D8:D15)=C16,NA(),C16-SUM(D8:D15)),NA())</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="9">
         <f>IFERROR(IF(D16-SUM(E8:E15)=D16,NA(),D16-SUM(E8:E15)),NA())</f>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="F16" s="9">
         <f>IFERROR(IF(E16-SUM(F8:F15)=E16,NA(),E16-SUM(F8:F15)),NA())</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" s="9">
         <f>IFERROR(IF(F16-SUM(G8:G15)=F16,NA(),F16-SUM(G8:G15)),NA())</f>
@@ -3776,59 +3776,59 @@
       </c>
       <c r="H16" s="9">
         <f>IFERROR(IF(G16-SUM(H8:H15)=G16,NA(),G16-SUM(H8:H15)),NA())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="9">
         <f>IFERROR(IF(H16-SUM(I8:I15)=H16,NA(),H16-SUM(I8:I15)),NA())</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="25">
+        <v>-1</v>
+      </c>
+      <c r="J16" s="24">
         <f>SUM(J8:J15)</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="22">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="21">
         <f>IFERROR(1-(J16/B16),"")</f>
-        <v>1</v>
+        <v>1.0333333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.5">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="37">
         <f>SUM(B8:B15)</f>
-        <v>31</v>
-      </c>
-      <c r="C17" s="11">
-        <f>IFERROR((IF(B17-($B$16/$G$4) &lt; 0,"-", B17-($B$16/$G$4))),IFERROR(B17-($B$16/20),"-"))</f>
-        <v>29.45</v>
-      </c>
-      <c r="D17" s="11">
-        <f>IFERROR((IF(C17-($B$16/$G$4) &lt; 0,"-", C17-($B$16/$G$4))),IFERROR(C17-($B$16/20),"-"))</f>
-        <v>27.9</v>
-      </c>
-      <c r="E17" s="11">
-        <f>IFERROR((IF(D17-($B$16/$G$4) &lt; 0,"-", D17-($B$16/$G$4))),IFERROR(D17-($B$16/20),"-"))</f>
-        <v>26.349999999999998</v>
-      </c>
-      <c r="F17" s="11">
-        <f>IFERROR((IF(E17-($B$16/$G$4) &lt; 0,"-", E17-($B$16/$G$4))),IFERROR(E17-($B$16/20),"-"))</f>
-        <v>24.799999999999997</v>
-      </c>
-      <c r="G17" s="11">
-        <f>IFERROR((IF(F17-($B$16/$G$4) &lt; 0,"-", F17-($B$16/$G$4))),IFERROR(F17-($B$16/20),"-"))</f>
-        <v>23.249999999999996</v>
-      </c>
-      <c r="H17" s="11">
-        <f>IFERROR((IF(G17-($B$16/$G$4) &lt; 0,"-", G17-($B$16/$G$4))),IFERROR(G17-($B$16/20),"-"))</f>
-        <v>21.699999999999996</v>
-      </c>
-      <c r="I17" s="11">
-        <f>IFERROR((IF(H17-($B$16/$G$4) &lt; 0,"-", H17-($B$16/$G$4))),IFERROR(H17-($B$16/20),"-"))</f>
-        <v>20.149999999999995</v>
-      </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
+        <v>30</v>
+      </c>
+      <c r="C17" s="10">
+        <f>IFERROR((IF(B17-($B$16/$G$4) &lt; 0,"-", B17-($B$16/$G$4))),IFERROR(B17-($B$16/7),"-"))</f>
+        <v>25.714285714285715</v>
+      </c>
+      <c r="D17" s="10">
+        <f>IFERROR((IF(C17-($B$16/$G$4) &lt; 0,"-", C17-($B$16/$G$4))),IFERROR(C17-($B$16/7),"-"))</f>
+        <v>21.428571428571431</v>
+      </c>
+      <c r="E17" s="10">
+        <f>IFERROR((IF(D17-($B$16/$G$4) &lt; 0,"-", D17-($B$16/$G$4))),IFERROR(D17-($B$16/7),"-"))</f>
+        <v>17.142857142857146</v>
+      </c>
+      <c r="F17" s="10">
+        <f>IFERROR((IF(E17-($B$16/$G$4) &lt; 0,"-", E17-($B$16/$G$4))),IFERROR(E17-($B$16/7),"-"))</f>
+        <v>12.857142857142861</v>
+      </c>
+      <c r="G17" s="10">
+        <f>IFERROR((IF(F17-($B$16/$G$4) &lt; 0,"-", F17-($B$16/$G$4))),IFERROR(F17-($B$16/7),"-"))</f>
+        <v>8.5714285714285765</v>
+      </c>
+      <c r="H17" s="10">
+        <f>IFERROR((IF(G17-($B$16/$G$4) &lt; 0,"-", G17-($B$16/$G$4))),IFERROR(G17-($B$16/7),"-"))</f>
+        <v>4.2857142857142909</v>
+      </c>
+      <c r="I17" s="10">
+        <f>IFERROR((IF(H17-($B$16/$G$4) &lt; 0,"-", H17-($B$16/$G$4))),IFERROR(H17-($B$16/7),"-"))</f>
+        <v>5.3290705182007514E-15</v>
+      </c>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3888,7 +3888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACA0E3D-6CA6-4BD2-BA12-8B619DAD9288}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>

</xml_diff>